<commit_message>
add more details in methods
</commit_message>
<xml_diff>
--- a/1_data/tables.xlsx
+++ b/1_data/tables.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill-my.sharepoint.com/personal/william_russell_mcgill_ca/Documents/Projects/generic-project/1_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jchen\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{7BC76095-3DD5-4ADC-A9C8-8CEF9F69B11E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AABEE5F0-D67E-A947-B9C8-A09D2CF4AB92}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="16000" xr2:uid="{FD511D9A-EB76-4ABE-81DE-0F0E048ADAAB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="sample" sheetId="1" r:id="rId1"/>
+    <sheet name="dataset" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>col1</t>
   </si>
@@ -55,12 +55,30 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Age Groups</t>
+  </si>
+  <si>
+    <t>18-35</t>
+  </si>
+  <si>
+    <t>36-64</t>
+  </si>
+  <si>
+    <t>65+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -405,68 +423,133 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D6B55D8-F496-4084-B55D-ABB6EB68893D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+      <c r="C3">
+        <v>33.33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+      <c r="C4">
+        <v>33.33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
+        <v>200</v>
+      </c>
+      <c r="C5">
+        <v>33.33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated methods section, tabs & figs
</commit_message>
<xml_diff>
--- a/1_data/tables.xlsx
+++ b/1_data/tables.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jchen\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill-my.sharepoint.com/personal/jiacheng_chen_mcgill_ca/Documents/APL/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25035" windowHeight="11505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="sample" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>col1</t>
   </si>
@@ -57,12 +57,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>%</t>
-  </si>
-  <si>
     <t>Age Groups</t>
   </si>
   <si>
@@ -73,6 +67,42 @@
   </si>
   <si>
     <t>65+</t>
+  </si>
+  <si>
+    <t>CBS</t>
+  </si>
+  <si>
+    <t>CANPATH</t>
+  </si>
+  <si>
+    <t>APL</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Provinces</t>
+  </si>
+  <si>
+    <t>Data Collecting Period</t>
+  </si>
+  <si>
+    <t>N (%)</t>
+  </si>
+  <si>
+    <t>200 (33.33%)</t>
+  </si>
+  <si>
+    <t>201 (33.33%)</t>
+  </si>
+  <si>
+    <t>202 (33.33%)</t>
   </si>
 </sst>
 </file>
@@ -108,8 +138,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,62 +525,94 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
-        <v>200</v>
-      </c>
-      <c r="C3">
-        <v>33.33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>200</v>
-      </c>
-      <c r="C4">
-        <v>33.33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5">
-        <v>200</v>
-      </c>
-      <c r="C5">
-        <v>33.33</v>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>